<commit_message>
Excel rules being corrected, 3.0.1
</commit_message>
<xml_diff>
--- a/dm-micro/src/main/resources/com/redhat/consulting/payment-review.xlsx
+++ b/dm-micro/src/main/resources/com/redhat/consulting/payment-review.xlsx
@@ -119,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t xml:space="preserve">RuleSet</t>
   </si>
@@ -136,7 +136,10 @@
     <t xml:space="preserve">Notes</t>
   </si>
   <si>
-    <t xml:space="preserve">RuleTable ID change</t>
+    <t xml:space="preserve">Checks if payments can be processed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RuleTable Payments</t>
   </si>
   <si>
     <t xml:space="preserve">CONDITION</t>
@@ -145,10 +148,13 @@
     <t xml:space="preserve">ACTION</t>
   </si>
   <si>
-    <t xml:space="preserve">paymaneVal : Double</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$param</t>
+    <t xml:space="preserve">$paymaneVal : Double</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$paymaneVal &gt;= $param </t>
+  </si>
+  <si>
+    <t xml:space="preserve">$paymaneVal &lt; $param </t>
   </si>
   <si>
     <t xml:space="preserve">System.out.println(The payment is $param);
@@ -158,25 +164,19 @@
     <t xml:space="preserve">Payment Rules</t>
   </si>
   <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Print</t>
+    <t xml:space="preserve">Payment Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Approval</t>
   </si>
   <si>
     <t xml:space="preserve">REJECTED PAYMENT</t>
   </si>
   <si>
-    <t xml:space="preserve">&gt;= 1000</t>
-  </si>
-  <si>
     <t xml:space="preserve">“REJECTED”</t>
   </si>
   <si>
     <t xml:space="preserve">APPROVED PAYMENT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt; 1000</t>
   </si>
   <si>
     <t xml:space="preserve">"APPROVED"</t>
@@ -676,7 +676,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2700" topLeftCell="A1" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
@@ -734,7 +734,9 @@
       <c r="B4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="10"/>
+      <c r="C4" s="10" t="s">
+        <v>5</v>
+      </c>
       <c r="D4" s="10"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -748,7 +750,7 @@
     <row r="6" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A6" s="12"/>
       <c r="B6" s="13" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="15"/>
@@ -759,40 +761,50 @@
       <c r="IS6" s="0"/>
       <c r="IU6" s="0"/>
     </row>
-    <row r="7" s="1" customFormat="true" ht="11" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="7" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A7" s="16"/>
       <c r="B7" s="17" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A8" s="16"/>
       <c r="B8" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="18"/>
+        <v>9</v>
+      </c>
+      <c r="C8" s="17"/>
+      <c r="D8" s="18"/>
     </row>
     <row r="9" s="22" customFormat="true" ht="28.85" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A9" s="19"/>
       <c r="B9" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="21" t="s">
         <v>10</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="23" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>15</v>
       </c>
       <c r="E10" s="1"/>
       <c r="IR10" s="0"/>
@@ -800,13 +812,16 @@
     </row>
     <row r="11" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="27" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="B11" s="27" t="n">
+        <v>1000</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>17</v>
       </c>
       <c r="E11" s="1"/>
       <c r="IR11" s="0"/>
@@ -814,12 +829,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="B12" s="27"/>
+      <c r="C12" s="28" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D12" s="28" t="s">
         <v>19</v>
       </c>
       <c r="E12" s="1"/>
@@ -836,8 +852,9 @@
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.15" right="0.140277777777778" top="0.179861111111111" bottom="0.2" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Adding XLSX defined rules and remotely executable via REST, 4.0.0
</commit_message>
<xml_diff>
--- a/dm-micro/src/main/resources/com/redhat/consulting/payment-review.xlsx
+++ b/dm-micro/src/main/resources/com/redhat/consulting/payment-review.xlsx
@@ -30,7 +30,7 @@
     <author> </author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -56,7 +56,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0">
+    <comment ref="B4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -85,7 +85,36 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0">
+    <comment ref="B5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Times New Roman"/>
+            <family val="1"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Look at me !!
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Times New Roman"/>
+            <family val="1"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">I tell you that I am a condition colmn. The next row down has the rule "template" and the row below that is a comment. After that, it is all rule data until an empty line !
+Note that if there is no data in a row, then this condition does not apply. 
+each row of rule data combines with a template to make a condition. Each row of rule data equates to a whole rule in a DRL file. 
+Other column types: ACTION, NAME, PRIORITY, DURATION - refer to http://drools.org/Decision+Tables for details</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -119,7 +148,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t xml:space="preserve">RuleSet</t>
   </si>
@@ -130,7 +159,8 @@
     <t xml:space="preserve">Import</t>
   </si>
   <si>
-    <t xml:space="preserve">java.lang.Double</t>
+    <t xml:space="preserve">java.lang.Double,
+com.redhat.consulting.domain.InFact</t>
   </si>
   <si>
     <t xml:space="preserve">Notes</t>
@@ -148,20 +178,74 @@
     <t xml:space="preserve">ACTION</t>
   </si>
   <si>
-    <t xml:space="preserve">$paymaneVal : Double</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$paymaneVal &gt;= $param </t>
-  </si>
-  <si>
-    <t xml:space="preserve">$paymaneVal &lt; $param </t>
-  </si>
-  <si>
-    <t xml:space="preserve">System.out.println(The payment is $param);
+    <t xml:space="preserve">$inFact : InFact()</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">$inFact.</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">getPaymentValue()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &gt;= ($param)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val=""/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">$inFact.</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val=""/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">getPaymentValue()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt; ($param)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">System.out.println("The payment is" + $param);
 insert($param);</t>
   </si>
   <si>
-    <t xml:space="preserve">Payment Rules</t>
+    <t xml:space="preserve">Rule Name</t>
   </si>
   <si>
     <t xml:space="preserve">Payment Value</t>
@@ -170,13 +254,13 @@
     <t xml:space="preserve">Approval</t>
   </si>
   <si>
-    <t xml:space="preserve">REJECTED PAYMENT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“REJECTED”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPROVED PAYMENT</t>
+    <t xml:space="preserve">REJECTING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"REJECTED"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPROVING</t>
   </si>
   <si>
     <t xml:space="preserve">"APPROVED"</t>
@@ -217,7 +301,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -269,6 +353,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="7"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Courier New"/>
@@ -281,6 +372,32 @@
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val=""/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val=""/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <name val=""/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val=""/>
+      <family val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -464,7 +581,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -477,39 +594,43 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -529,7 +650,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -541,11 +662,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -557,11 +682,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="10" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -569,15 +694,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -585,11 +710,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -671,20 +796,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:IU14"/>
+  <dimension ref="A1:IU1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2700" topLeftCell="A1" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="2295" topLeftCell="A1" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="27.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="31.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="19.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.64"/>
@@ -695,166 +820,155 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="258" style="0" width="9.13"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5"/>
+      <c r="E1" s="6"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
       <c r="IU1" s="0"/>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="B2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="3"/>
+    <row r="2" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="IU2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="B3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="3"/>
-      <c r="G3" s="7"/>
+      <c r="B3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="11"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
       <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
+      <c r="I3" s="12"/>
       <c r="IU3" s="0"/>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="B4" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="11"/>
+    <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A4" s="13"/>
+      <c r="B4" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="IR4" s="0"/>
+      <c r="IS4" s="0"/>
       <c r="IU4" s="0"/>
     </row>
-    <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="IU5" s="0"/>
-    </row>
-    <row r="6" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="IR6" s="0"/>
-      <c r="IS6" s="0"/>
-      <c r="IU6" s="0"/>
-    </row>
-    <row r="7" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A7" s="16"/>
-      <c r="B7" s="17" t="s">
+    <row r="5" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A5" s="17"/>
+      <c r="B5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C5" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="A8" s="16"/>
-      <c r="B8" s="17" t="s">
+    </row>
+    <row r="6" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A6" s="17"/>
+      <c r="B6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="18"/>
-    </row>
-    <row r="9" s="22" customFormat="true" ht="28.85" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A9" s="19"/>
-      <c r="B9" s="20" t="s">
+      <c r="C6" s="18"/>
+      <c r="D6" s="19"/>
+    </row>
+    <row r="7" s="24" customFormat="true" ht="28.85" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="A7" s="20"/>
+      <c r="B7" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C7" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D7" s="23" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="23" t="s">
+    <row r="8" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B8" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C8" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D8" s="27" t="s">
         <v>15</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="IR8" s="0"/>
+      <c r="IS8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="29" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="IR9" s="0"/>
+      <c r="IS9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>19</v>
       </c>
       <c r="E10" s="1"/>
       <c r="IR10" s="0"/>
       <c r="IS10" s="0"/>
     </row>
-    <row r="11" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="27" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C11" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="28" t="s">
-        <v>17</v>
-      </c>
+    <row r="11" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="31"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="30"/>
       <c r="E11" s="1"/>
       <c r="IR11" s="0"/>
       <c r="IS11" s="0"/>
     </row>
-    <row r="12" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="28" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D12" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="IR12" s="0"/>
-      <c r="IS12" s="0"/>
-    </row>
-    <row r="13" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="29"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="28"/>
-      <c r="E13" s="1"/>
-      <c r="IR13" s="0"/>
-      <c r="IS13" s="0"/>
-    </row>
-    <row r="14" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B8:C8"/>
+  <mergeCells count="1">
+    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.15" right="0.140277777777778" top="0.179861111111111" bottom="0.2" header="0.511805555555555" footer="0.511805555555555"/>
@@ -900,35 +1014,35 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="33" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="33" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="33" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changes to be able to extract results via global variable resultsList, bash scripts to be updated
</commit_message>
<xml_diff>
--- a/dm-micro/src/main/resources/com/redhat/consulting/payment-review.xlsx
+++ b/dm-micro/src/main/resources/com/redhat/consulting/payment-review.xlsx
@@ -177,15 +177,20 @@
         <color rgb="FFFFFFFF"/>
         <rFont val="Monospace"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">com.redhat.consulting.domain.OutResults</t>
+      <t xml:space="preserve">com.redhat.consulting.domain.OutResults,
+java.util.</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Variables</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OutResults outResult</t>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">ArrayList</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Notes</t>
@@ -268,120 +273,64 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">System.out.println("Executing for inFact [" + $inFact + "]");
+System.out.println("The payment is " + $param);
+resultsList.add($param);
+System.out.println("The out Array is " + resultsList);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rule Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payment Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Approval</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REJECTING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"REJECTED"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APPROVING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"APPROVED"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variables</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="7"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="1"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
       </rPr>
-      <t xml:space="preserve">System.out.println("The payment is" + $param);
-</t>
+      <t xml:space="preserve">java.util.ArrayList</t>
     </r>
     <r>
       <rPr>
         <sz val="7"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FF000000"/>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF2A00FF"/>
         <rFont val="Monospace"/>
         <family val="0"/>
       </rPr>
-      <t xml:space="preserve">//if (outResult == null) {outResult = new OutResults(); }
-//outResult.</t>
+      <t xml:space="preserve">resultsList</t>
     </r>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="7"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Monospace"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">addApproval(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Monospace"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">$param);
-//</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">insert(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Monospace"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">outResult</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">);
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">insert(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Monospace"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">$param</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">);</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Rule Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Payment Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Approval</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REJECTING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"REJECTED"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APPROVING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"APPROVED"</t>
   </si>
   <si>
     <t xml:space="preserve">Insurance Types</t>
@@ -419,7 +368,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="25">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -482,6 +431,13 @@
       <color rgb="FFFFFFFF"/>
       <name val="Monospace"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Monospace"/>
+      <family val="0"/>
     </font>
     <font>
       <b val="true"/>
@@ -496,6 +452,11 @@
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -526,24 +487,38 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
-      <sz val="7"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Monospace"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="7"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Monospace"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF000000"/>
+      <name val="Monospace"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Monospace"/>
+      <family val="0"/>
     </font>
     <font>
       <b val="true"/>
@@ -561,7 +536,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -572,6 +547,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF000000"/>
         <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -602,6 +583,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFAA61A"/>
+        <bgColor rgb="FFFFCC00"/>
       </patternFill>
     </fill>
   </fills>
@@ -663,16 +656,10 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FFDADADA"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFDADADA"/>
-      </right>
-      <top style="thin"/>
-      <bottom style="thin">
-        <color rgb="FFDADADA"/>
-      </bottom>
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -719,7 +706,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="41">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -756,67 +743,71 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="16" fillId="5" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -824,39 +815,59 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="5" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="12" fillId="7" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="12" fillId="8" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="9" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="9" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="19" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="20" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -903,7 +914,7 @@
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF2A00FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
@@ -916,7 +927,7 @@
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFAA61A"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
@@ -938,20 +949,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:IU1048576"/>
+  <dimension ref="A1:AMJ14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2295" topLeftCell="A1" activePane="bottomLeft" state="split"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
       <selection pane="bottomLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="27.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="33.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="31.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="35.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="19.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.64"/>
@@ -990,14 +1001,10 @@
       <c r="I2" s="7"/>
       <c r="IU2" s="0"/>
     </row>
-    <row r="3" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="5"/>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="B3" s="0"/>
+      <c r="C3" s="0"/>
+      <c r="D3" s="9"/>
       <c r="E3" s="6"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -1006,10 +1013,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B4" s="10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="6"/>
@@ -1018,10 +1025,10 @@
       <c r="I4" s="13"/>
       <c r="IU4" s="0"/>
     </row>
-    <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A5" s="14"/>
       <c r="B5" s="15" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="17"/>
@@ -1035,92 +1042,102 @@
     <row r="6" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A6" s="18"/>
       <c r="B6" s="19" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>10</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="AMJ6" s="0"/>
     </row>
     <row r="7" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A7" s="18"/>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="20"/>
+      <c r="AMJ7" s="0"/>
+    </row>
+    <row r="8" s="26" customFormat="true" ht="46.65" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="A8" s="22"/>
+      <c r="B8" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="20"/>
-    </row>
-    <row r="8" s="25" customFormat="true" ht="48.35" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="A8" s="21"/>
-      <c r="B8" s="22" t="s">
+      <c r="D8" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="AMJ8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="B9" s="28" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="26" t="s">
+      <c r="C9" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="29" t="s">
         <v>15</v>
-      </c>
-      <c r="B9" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="28" t="s">
-        <v>17</v>
       </c>
       <c r="E9" s="1"/>
       <c r="IR9" s="0"/>
       <c r="IS9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="30" t="n">
+      <c r="A10" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="31" t="n">
         <v>1000</v>
       </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31" t="s">
-        <v>19</v>
+      <c r="C10" s="32"/>
+      <c r="D10" s="33" t="s">
+        <v>17</v>
       </c>
       <c r="E10" s="1"/>
       <c r="IR10" s="0"/>
       <c r="IS10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="31" t="n">
+      <c r="A11" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="34"/>
+      <c r="C11" s="33" t="n">
         <v>1000</v>
       </c>
-      <c r="D11" s="31" t="s">
-        <v>21</v>
+      <c r="D11" s="33" t="s">
+        <v>19</v>
       </c>
       <c r="E11" s="1"/>
       <c r="IR11" s="0"/>
       <c r="IS11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="32"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="31"/>
+      <c r="A12" s="35"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="37"/>
       <c r="E12" s="1"/>
       <c r="IR12" s="0"/>
       <c r="IS12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="39" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B7:C7"/>
@@ -1143,7 +1160,7 @@
   </sheetPr>
   <dimension ref="A4:E7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1169,35 +1186,35 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="34" t="s">
+      <c r="E5" s="40" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="34" t="s">
+      <c r="E6" s="40" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="34" t="s">
+      <c r="E7" s="40" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>